<commit_message>
add mulfiwfn data reader
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="846" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="846" firstSheet="10" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -28,15 +28,21 @@
     <sheet name="pbe0 S1_energy" sheetId="14" r:id="rId14"/>
     <sheet name="pbe0 T1_energy" sheetId="15" r:id="rId15"/>
     <sheet name="pbe0 delta_E_S1_T1" sheetId="16" r:id="rId16"/>
-    <sheet name="pbe0 T1_S1_SOCME" sheetId="17" r:id="rId17"/>
-    <sheet name="pbe0 T1_S2_SOCME" sheetId="18" r:id="rId18"/>
+    <sheet name="pbe0 delta_E_S2_T1" sheetId="17" r:id="rId17"/>
+    <sheet name="pbe0 T1_S1_SOCME" sheetId="18" r:id="rId18"/>
+    <sheet name="pbe0 T1_S2_SOCME" sheetId="19" r:id="rId19"/>
+    <sheet name="pbe0 T1_S1_kRISC" sheetId="23" r:id="rId20"/>
+    <sheet name="pbe0 T1_S2_kRISC" sheetId="24" r:id="rId21"/>
+    <sheet name="pbe0 distance" sheetId="20" r:id="rId22"/>
+    <sheet name="pbe0 integral_norm" sheetId="21" r:id="rId23"/>
+    <sheet name="pbe0 integral_square" sheetId="22" r:id="rId24"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
@@ -98,6 +104,9 @@
     <t>HOMO energies, eV (PBE0/def2-TZVP, CPCM(toluene))</t>
   </si>
   <si>
+    <t>mean</t>
+  </si>
+  <si>
     <t>LUMO energies, eV (PBE0/def2-TZVP, CPCM(toluene))</t>
   </si>
   <si>
@@ -113,10 +122,31 @@
     <t>ΔE(S1-T1), eV (PBE0/def2-TZVP, CPCM(toluene))</t>
   </si>
   <si>
+    <t>ΔE(S2-T1), eV (PBE0/def2-TZVP, CPCM(toluene))</t>
+  </si>
+  <si>
     <t>Spin-Orbit Coupling Matrix Element for S1 and T1, cm-1 (PBE0/def2-TZVP, CPCM(toluene))</t>
   </si>
   <si>
     <t>Spin-Orbit Coupling between T1 and S2, cm-1 (PBE0/def2-TZVP, CPCM(toluene))</t>
+  </si>
+  <si>
+    <t>Distance between centroids of HOMO and LUMO (PBE0/def2-TZVP, CPCM(toluene)), Angstrom</t>
+  </si>
+  <si>
+    <t>Overlap integral for module of HOMO and LUMO (PBE0/def2-TZVP, CPCM(toluene))</t>
+  </si>
+  <si>
+    <t>Overlap integral for squared HOMO and LUMO (PBE0/def2-TZVP, CPCM(toluene))</t>
+  </si>
+  <si>
+    <t>(SOCME(T1-S1))^2*exp(-ΔE(S1-T1)^2) (PBE0/def2-TZVP, CPCM(toluene))</t>
+  </si>
+  <si>
+    <t>(SOCME(T1-S2))^2*exp(-ΔE(S2-T1)^2) (PBE0/def2-TZVP, CPCM(toluene))</t>
+  </si>
+  <si>
+    <t>Подсвечено зеленым если соответствующее значение dE(ST) &lt; 0.3</t>
   </si>
 </sst>
 </file>
@@ -126,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +180,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -260,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -278,6 +315,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -301,13 +339,64 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99CC"/>
+      <color rgb="FFCCFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -618,18 +707,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -809,7 +898,7 @@
   <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,18 +907,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -1150,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M12"/>
+  <dimension ref="B2:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,21 +1250,21 @@
     <col min="2" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1187,7 +1276,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1216,8 +1305,11 @@
       <c r="K4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1252,8 +1344,12 @@
         <f t="shared" ref="M5:M12" si="0">MAX(C5:K5)-MIN(C5:K5)</f>
         <v>0.21480000000000032</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="7">
+        <f t="shared" ref="O5:O12" si="1">AVERAGE(C5:K5)</f>
+        <v>-5.9092888888888888</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1288,8 +1384,12 @@
         <f t="shared" si="0"/>
         <v>0.31119999999999948</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="7">
+        <f t="shared" si="1"/>
+        <v>-5.7721111111111112</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1324,8 +1424,12 @@
         <f t="shared" si="0"/>
         <v>0.24500000000000011</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="7">
+        <f t="shared" si="1"/>
+        <v>-5.4216999999999986</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1360,8 +1464,12 @@
         <f t="shared" si="0"/>
         <v>0.30269999999999975</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="7">
+        <f t="shared" si="1"/>
+        <v>-5.4427555555555562</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1396,8 +1504,12 @@
         <f t="shared" si="0"/>
         <v>0.18880000000000052</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="7">
+        <f t="shared" si="1"/>
+        <v>-5.6182888888888893</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1432,8 +1544,12 @@
         <f t="shared" si="0"/>
         <v>0.17740000000000045</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="7">
+        <f t="shared" si="1"/>
+        <v>-5.4785333333333339</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
@@ -1464,12 +1580,16 @@
       <c r="K11" s="6">
         <v>-5.1703999999999999</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="7">
         <f t="shared" si="0"/>
         <v>0.19329999999999981</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="7">
+        <f t="shared" si="1"/>
+        <v>-5.263066666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>8</v>
       </c>
@@ -1500,9 +1620,13 @@
       <c r="K12" s="6">
         <v>-5.9786000000000001</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="7">
         <f t="shared" si="0"/>
         <v>0.21170000000000044</v>
+      </c>
+      <c r="O12" s="7">
+        <f t="shared" si="1"/>
+        <v>-6.031477777777777</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1634,7 @@
     <mergeCell ref="B2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:K12">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1520,12 +1644,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M12">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:O12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1538,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,18 +1682,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -1860,39 +1994,39 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="16">
-        <f>-MIN(C5:C12)+MAX(C5:C12)</f>
+      <c r="C15" s="7">
+        <f t="shared" ref="C15:K15" si="0">-MIN(C5:C12)+MAX(C5:C12)</f>
         <v>0.3044</v>
       </c>
-      <c r="D15" s="16">
-        <f t="shared" ref="D15:K15" si="0">-MIN(D5:D12)+MAX(D5:D12)</f>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
         <v>0.15339999999999998</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="7">
         <f t="shared" si="0"/>
         <v>0.10899999999999999</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="7">
         <f t="shared" si="0"/>
         <v>0.17320000000000002</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
         <v>0.1944999999999999</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>0.21310000000000007</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="7">
         <f t="shared" si="0"/>
         <v>0.10579999999999989</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="7">
         <f t="shared" si="0"/>
         <v>0.12250000000000005</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="7">
         <f t="shared" si="0"/>
         <v>8.2599999999999785E-2</v>
       </c>
@@ -1928,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K12"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="M5" sqref="M5:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,21 +2073,21 @@
     <col min="2" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1965,7 +2099,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1995,7 +2129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2026,8 +2160,12 @@
       <c r="K5" s="6">
         <v>3.2292000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="7">
+        <f t="shared" ref="M5:M12" si="0">AVERAGE(C5:K5)</f>
+        <v>3.8803666666666663</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -2058,8 +2196,12 @@
       <c r="K6" s="6">
         <v>3.1248999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="7">
+        <f t="shared" si="0"/>
+        <v>3.8503222222222218</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -2090,8 +2232,12 @@
       <c r="K7" s="6">
         <v>2.7778999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="7">
+        <f t="shared" si="0"/>
+        <v>3.4810888888888889</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -2122,8 +2268,12 @@
       <c r="K8" s="6">
         <v>2.7955999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="7">
+        <f t="shared" si="0"/>
+        <v>3.5544999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -2154,8 +2304,12 @@
       <c r="K9" s="6">
         <v>2.9504999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="7">
+        <f t="shared" si="0"/>
+        <v>3.5996111111111113</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -2186,8 +2340,12 @@
       <c r="K10" s="6">
         <v>2.8026</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="7">
+        <f t="shared" si="0"/>
+        <v>3.4352555555555551</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
@@ -2218,8 +2376,12 @@
       <c r="K11" s="6">
         <v>2.5764</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="7">
+        <f t="shared" si="0"/>
+        <v>3.212822222222222</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>8</v>
       </c>
@@ -2249,6 +2411,10 @@
       </c>
       <c r="K12" s="6">
         <v>3.4102000000000001</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" si="0"/>
+        <v>4.0403222222222226</v>
       </c>
     </row>
   </sheetData>
@@ -2275,7 +2441,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M11">
+  <conditionalFormatting sqref="M5:M12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2304,7 +2470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2312,18 +2480,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -2656,18 +2824,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -2988,10 +3156,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K12"/>
+  <dimension ref="B2:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="S5" sqref="S5:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2999,19 +3167,711 @@
     <col min="2" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:23" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.39257886780000018</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.45086568659999982</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.2277594179999998</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.53119373939999992</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.51383286619999957</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.67718290040000051</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.5401652400000019E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.24370529839999969</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.31801963179999992</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:U12" si="0">IF(C5&lt;0.3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ref="W5:W12" si="1">AVERAGE(C5:K5)</f>
+        <v>0.37450445122222215</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.61293678500000048</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.55611938179999987</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.38272834100000003</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.65046130559999993</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.58942613539999966</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.68159114720000025</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3.074888200000014E-2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.32395171699999992</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.16653376799999989</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="1"/>
+        <v>0.44383305144444446</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.34392488460000031</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.2118951718000002</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5.5484044600000448E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.39032032160000002</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.25390957340000009</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.44330091740000022</v>
+      </c>
+      <c r="I7" s="3">
+        <v>4.571515199999876E-3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>9.3307890599999777E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>7.0749640000000724E-4</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="1"/>
+        <v>0.19971353506666678</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.43059319359999998</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.25943348760000001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.10881838859999959</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.43851171099999992</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.30721670599999967</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.51356075220000008</v>
+      </c>
+      <c r="I8" s="3">
+        <v>9.5239899999999267E-3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.15317297060000001</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1.496626999999862E-3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="1"/>
+        <v>0.24692531406666657</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3.7143561000000158E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.17469718800000009</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5.4422800000031302E-4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.15001644820000021</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.26623633760000009</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.32776131300000028</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5.4422799999898068E-5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>4.6259380000002182E-4</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4.2939589200000412E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="1"/>
+        <v>0.11109507573333349</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9.4369135199999565E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.14582589260000001</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.8775866000000361E-3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.18824846519999999</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.2121400744000006</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.28890343380000028</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.7211399999949041E-5</v>
+      </c>
+      <c r="J10" s="3">
+        <v>5.4422800000031302E-4</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2.7211399999949041E-5</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="1"/>
+        <v>0.10355147095555564</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5.9348063399999873E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5.5565678799999851E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.1700902000000291E-3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.1069952248000003</v>
+      </c>
+      <c r="G11" s="3">
+        <v>9.2518760000000366E-2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.17954081719999951</v>
+      </c>
+      <c r="I11" s="3">
+        <v>5.4422800000342157E-5</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2.9932540000032759E-4</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2.721140000039313E-5</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="1"/>
+        <v>5.5057732666666775E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.6111136211999999</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.58773902859999971</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.35165292220000038</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.69032600659999988</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.64069241300000046</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.80600166799999995</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4.8953308599999801E-2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.38286439799999972</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.46240332020000002</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="1"/>
+        <v>0.50908296515555551</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:K12">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:U12 W5:W12">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W5:W12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:U12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -3060,31 +3920,31 @@
         <v>1</v>
       </c>
       <c r="C5" s="3">
-        <v>0.39257886780000018</v>
+        <v>0.41437519920000021</v>
       </c>
       <c r="D5" s="3">
-        <v>0.45086568659999982</v>
+        <v>0.49619987899999968</v>
       </c>
       <c r="E5" s="3">
-        <v>0.2277594179999998</v>
+        <v>0.23037171239999979</v>
       </c>
       <c r="F5" s="3">
-        <v>0.53119373939999992</v>
+        <v>0.54371098340000046</v>
       </c>
       <c r="G5" s="3">
-        <v>0.51383286619999957</v>
+        <v>0.57595649239999958</v>
       </c>
       <c r="H5" s="3">
-        <v>0.67718290040000051</v>
+        <v>0.68439392140000033</v>
       </c>
       <c r="I5" s="3">
-        <v>1.5401652400000019E-2</v>
+        <v>1.7524141599999599E-2</v>
       </c>
       <c r="J5" s="3">
-        <v>0.24370529839999969</v>
+        <v>0.30865891019999969</v>
       </c>
       <c r="K5" s="3">
-        <v>0.31801963179999992</v>
+        <v>0.31845501419999961</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3092,31 +3952,31 @@
         <v>2</v>
       </c>
       <c r="C6" s="3">
-        <v>0.61293678500000048</v>
+        <v>0.62485537820000037</v>
       </c>
       <c r="D6" s="3">
-        <v>0.55611938179999987</v>
+        <v>0.62880103120000008</v>
       </c>
       <c r="E6" s="3">
-        <v>0.38272834100000003</v>
+        <v>0.38368074000000002</v>
       </c>
       <c r="F6" s="3">
-        <v>0.65046130559999993</v>
+        <v>0.65269264039999975</v>
       </c>
       <c r="G6" s="3">
-        <v>0.58942613539999966</v>
+        <v>0.66945486279999944</v>
       </c>
       <c r="H6" s="3">
-        <v>0.68159114720000025</v>
+        <v>0.68692458160000003</v>
       </c>
       <c r="I6" s="3">
-        <v>3.074888200000014E-2</v>
+        <v>3.2789737000000319E-2</v>
       </c>
       <c r="J6" s="3">
-        <v>0.32395171699999992</v>
+        <v>0.43018502259999991</v>
       </c>
       <c r="K6" s="3">
-        <v>0.16653376799999989</v>
+        <v>0.1670507846000002</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3124,31 +3984,31 @@
         <v>3</v>
       </c>
       <c r="C7" s="3">
-        <v>0.34392488460000031</v>
+        <v>0.40378996460000011</v>
       </c>
       <c r="D7" s="3">
-        <v>0.2118951718000002</v>
+        <v>0.2777467598000003</v>
       </c>
       <c r="E7" s="3">
-        <v>5.5484044600000448E-2</v>
+        <v>5.6953460200000361E-2</v>
       </c>
       <c r="F7" s="3">
-        <v>0.39032032160000002</v>
+        <v>0.41793989259999981</v>
       </c>
       <c r="G7" s="3">
-        <v>0.25390957340000009</v>
+        <v>0.34340786800000028</v>
       </c>
       <c r="H7" s="3">
-        <v>0.44330091740000022</v>
+        <v>0.45872978119999969</v>
       </c>
       <c r="I7" s="3">
-        <v>4.571515199999876E-3</v>
+        <v>6.1225650000000797E-3</v>
       </c>
       <c r="J7" s="3">
-        <v>9.3307890599999777E-2</v>
+        <v>0.18155446079999971</v>
       </c>
       <c r="K7" s="3">
-        <v>7.0749640000000724E-4</v>
+        <v>9.5239899999999267E-4</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3156,31 +4016,31 @@
         <v>4</v>
       </c>
       <c r="C8" s="3">
-        <v>0.43059319359999998</v>
+        <v>0.55813302540000009</v>
       </c>
       <c r="D8" s="3">
-        <v>0.25943348760000001</v>
+        <v>0.34055067100000042</v>
       </c>
       <c r="E8" s="3">
-        <v>0.10881838859999959</v>
+        <v>0.11355317219999959</v>
       </c>
       <c r="F8" s="3">
-        <v>0.43851171099999992</v>
+        <v>0.52664943560000044</v>
       </c>
       <c r="G8" s="3">
-        <v>0.30721670599999967</v>
+        <v>0.42637542660000038</v>
       </c>
       <c r="H8" s="3">
-        <v>0.51356075220000008</v>
+        <v>0.58806556539999955</v>
       </c>
       <c r="I8" s="3">
-        <v>9.5239899999999267E-3</v>
+        <v>1.687106799999993E-2</v>
       </c>
       <c r="J8" s="3">
-        <v>0.15317297060000001</v>
+        <v>0.25249458060000007</v>
       </c>
       <c r="K8" s="3">
-        <v>1.496626999999862E-3</v>
+        <v>1.2245129999999721E-2</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3188,31 +4048,31 @@
         <v>5</v>
       </c>
       <c r="C9" s="3">
-        <v>3.7143561000000158E-2</v>
+        <v>5.1320700400000252E-2</v>
       </c>
       <c r="D9" s="3">
-        <v>0.17469718800000009</v>
+        <v>0.17486045640000031</v>
       </c>
       <c r="E9" s="3">
-        <v>5.4422800000031302E-4</v>
+        <v>4.1905556000001454E-3</v>
       </c>
       <c r="F9" s="3">
-        <v>0.15001644820000021</v>
+        <v>0.15238384000000019</v>
       </c>
       <c r="G9" s="3">
-        <v>0.26623633760000009</v>
+        <v>0.26800507860000028</v>
       </c>
       <c r="H9" s="3">
-        <v>0.32776131300000028</v>
+        <v>0.3292035172000003</v>
       </c>
       <c r="I9" s="3">
-        <v>5.4422799999898068E-5</v>
+        <v>1.5510497999997601E-3</v>
       </c>
       <c r="J9" s="3">
-        <v>4.6259380000002182E-4</v>
+        <v>5.115743200000189E-3</v>
       </c>
       <c r="K9" s="3">
-        <v>4.2939589200000412E-2</v>
+        <v>4.3402182999999983E-2</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3220,31 +4080,31 @@
         <v>6</v>
       </c>
       <c r="C10" s="3">
-        <v>9.4369135199999565E-2</v>
+        <v>0.1201383309999997</v>
       </c>
       <c r="D10" s="3">
-        <v>0.14582589260000001</v>
+        <v>0.14658781179999991</v>
       </c>
       <c r="E10" s="3">
-        <v>1.8775866000000361E-3</v>
+        <v>6.0409307999997894E-3</v>
       </c>
       <c r="F10" s="3">
-        <v>0.18824846519999999</v>
+        <v>0.19706495880000041</v>
       </c>
       <c r="G10" s="3">
-        <v>0.2121400744000006</v>
+        <v>0.21619457300000011</v>
       </c>
       <c r="H10" s="3">
-        <v>0.28890343380000028</v>
+        <v>0.28925718200000011</v>
       </c>
       <c r="I10" s="3">
-        <v>2.7211399999949041E-5</v>
+        <v>5.2245888000004292E-3</v>
       </c>
       <c r="J10" s="3">
-        <v>5.4422800000031302E-4</v>
+        <v>4.7347836000004584E-3</v>
       </c>
       <c r="K10" s="3">
-        <v>2.7211399999949041E-5</v>
+        <v>3.8912301999993741E-3</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3252,31 +4112,31 @@
         <v>7</v>
       </c>
       <c r="C11" s="3">
-        <v>5.9348063399999873E-2</v>
+        <v>6.7266580799999698E-2</v>
       </c>
       <c r="D11" s="3">
-        <v>5.5565678799999851E-2</v>
+        <v>6.3647464600000259E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>1.1700902000000291E-3</v>
+        <v>1.697991359999973E-2</v>
       </c>
       <c r="F11" s="3">
-        <v>0.1069952248000003</v>
+        <v>0.1146144168000003</v>
       </c>
       <c r="G11" s="3">
-        <v>9.2518760000000366E-2</v>
+        <v>9.6382778800000235E-2</v>
       </c>
       <c r="H11" s="3">
-        <v>0.17954081719999951</v>
+        <v>0.1853368453999997</v>
       </c>
       <c r="I11" s="3">
-        <v>5.4422800000342157E-5</v>
+        <v>2.1333737600000461E-2</v>
       </c>
       <c r="J11" s="3">
-        <v>2.9932540000032759E-4</v>
+        <v>1.175532480000019E-2</v>
       </c>
       <c r="K11" s="3">
-        <v>2.721140000039313E-5</v>
+        <v>6.0409308000002326E-3</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3284,31 +4144,31 @@
         <v>8</v>
       </c>
       <c r="C12" s="3">
-        <v>0.6111136211999999</v>
+        <v>0.67544137079999977</v>
       </c>
       <c r="D12" s="3">
-        <v>0.58773902859999971</v>
+        <v>0.63870598080000018</v>
       </c>
       <c r="E12" s="3">
-        <v>0.35165292220000038</v>
+        <v>0.37067369080000029</v>
       </c>
       <c r="F12" s="3">
-        <v>0.69032600659999988</v>
+        <v>0.71489790080000049</v>
       </c>
       <c r="G12" s="3">
-        <v>0.64069241300000046</v>
+        <v>0.69658462860000059</v>
       </c>
       <c r="H12" s="3">
-        <v>0.80600166799999995</v>
+        <v>0.81590661760000005</v>
       </c>
       <c r="I12" s="3">
-        <v>4.8953308599999801E-2</v>
+        <v>5.5075873599999881E-2</v>
       </c>
       <c r="J12" s="3">
-        <v>0.38286439799999972</v>
+        <v>0.45995429419999972</v>
       </c>
       <c r="K12" s="3">
-        <v>0.46240332020000002</v>
+        <v>0.48077101519999982</v>
       </c>
     </row>
   </sheetData>
@@ -3330,12 +4190,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3344,18 +4204,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -3684,7 +4544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K12"/>
   <sheetViews>
@@ -3698,18 +4558,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -4042,18 +4902,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -4372,6 +5232,2280 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:U15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.3480200700264062E-11</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6.7736180652928524E-11</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.9404451716791198E-10</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2.5155127585623731E-10</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.620589429697503E-10</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2.3613437932278792E-10</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.137205549168761E-10</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2.3465593781457342E-10</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2.784100890315066E-9</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:U12" si="0">-LOG10(C5)</f>
+        <v>10.361708459921161</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>10.169179294968046</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>9.4044547109961805</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>9.5993734756114648</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>9.5816010150640647</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>9.6268407784306955</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>9.9441610297699423</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>9.6295684517754729</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>8.5553150308024257</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.3284597181746698E-11</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.105662618510534E-10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4.1822013805561941E-10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.01690805499422E-10</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.4009286433765221E-10</v>
+      </c>
+      <c r="H6" s="3">
+        <v>8.0173288636100667E-11</v>
+      </c>
+      <c r="I6" s="3">
+        <v>6.6648346092628612E-10</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3.3630988527602438E-10</v>
+      </c>
+      <c r="K6" s="3">
+        <v>9.888489488884315E-9</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>10.363666619790648</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>9.956377373277137</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>9.3785950589505216</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>9.9927183125775603</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>9.8535839850404532</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>10.095970301668689</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>9.1762106233207472</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>9.4732603671256435</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>8.0048700437661999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.2837128641075049E-10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.74822473187555E-10</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.7583273677333189E-11</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.441840283986711E-9</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.4411569271886451E-11</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4.9252603388558203E-10</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.3833870411262759E-11</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3.8095103109416918E-11</v>
+      </c>
+      <c r="K7" s="3">
+        <v>6.1485122667543083E-12</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>9.8915321067025275</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>9.5609477563931229</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>10.55935419154561</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>8.6122827458176996</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>10.841288726402253</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>9.3075708086708762</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>10.859056296890467</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>10.419130846614131</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>11.211229956176098</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.679241916497334E-9</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0921778211540311E-10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6.1065181207289523E-10</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3.5764140929295692E-10</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.251886611082736E-10</v>
+      </c>
+      <c r="H8" s="3">
+        <v>8.230006979237727E-10</v>
+      </c>
+      <c r="I8" s="3">
+        <v>5.3794629525787003E-11</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.711692398194459E-10</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2.6131131682711791E-11</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>8.7748867336227203</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>9.9617066469253785</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>9.2142063498199889</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>9.4465522024424864</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>9.647453481236699</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>9.0845997964957323</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>10.269261079049885</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>9.7665742780756339</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>10.582841781512082</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.7630172936090089E-11</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.1117154071655355E-10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3.0742567616538439E-12</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.1912605744349888E-9</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6.5010357394283357E-10</v>
+      </c>
+      <c r="H9" s="3">
+        <v>8.2005230532327708E-10</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.537128507165188E-12</v>
+      </c>
+      <c r="K9" s="3">
+        <v>7.6714863819546458E-12</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>10.558616396844089</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>9.1480256310550789</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>11.512259863084601</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>8.6593059751045676</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>9.1870174464210876</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>9.0861584461665093</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>11.813289823053445</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>11.115120481560789</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4.4181519043044412E-11</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6.7715396936393025E-10</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2.1519727841093129E-11</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.5221382421992372E-11</v>
+      </c>
+      <c r="G10" s="3">
+        <v>8.5524101722619274E-10</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2.4038685636148099E-11</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3.0742567616538439E-12</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>10.35475935635343</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>9.1693125714294386</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>10.66716322547121</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>10.598231112775276</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>9.0679114786039747</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>10.619089281951046</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>11.512259863084601</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8.1181387674568611E-11</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7.2022339461442666E-10</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7.6856336580066296E-12</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.033349869253619E-10</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1.292375399438991E-9</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2.5897633278459032E-10</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>10.090543529339785</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>9.1425327757904249</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>11.114320320378823</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>9.9857526111420292</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>8.8886113174367996</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>9.5867399232187687</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>9.0518787555824178E-9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.290654859324672E-8</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.404513925648219E-9</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2.2686011462478761E-8</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.3806667616096451E-8</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2.814331790690353E-8</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.3571029227054929E-9</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.5082235200976451E-8</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>8.0432612717891345</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>7.8891898791361958</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>8.8524739504444625</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>7.6442418528193672</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>7.859911130297518</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>7.550624703499806</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>8.8673872141913765</v>
+      </c>
+      <c r="T12">
+        <f>-LOG10(J12)</f>
+        <v>7.8215342908591809</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="M5:U12">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="between">
+      <formula>10</formula>
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="2" priority="7">
+      <formula>LEN(TRIM(M5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{9A9DF85B-55A5-4545-801B-D1A8F95AD5CD}">
+            <xm:f>'pbe0 delta_E_S1_T1'!C5&lt;0.3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCCFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C5:K12</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:U12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5.1900914221931506E-9</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.2362848545539038E-9</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4.0086161016463938E-10</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3.3282536328672601E-9</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3.5246371360301038E-9</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.9812771708375489E-9</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4.154605613666505E-9</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:U12" si="0">-LOG10(C5)</f>
+        <v>8.284824992092906</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>8.650472877493339</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>9.3970055334027105</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>8.477783585278706</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>8.452885587305639</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>8.7030547645699574</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>8.3814701964136127</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.4342117070362021E-10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5.5793424682749907E-10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>6.7131739510956916E-10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.8148817494376023E-11</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.8361755474009481E-10</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1.515091374544085E-10</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.535477054257021E-12</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2.395197737040603E-9</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.494826758468606E-12</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>9.6136416532221141</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>9.2534169801352011</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>9.1730720992738615</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>10.418518919403114</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>9.7360858004642949</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>9.8195611742484008</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>11.813756669148635</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>8.6206586273180079</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>11.82540913657083</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.7165077418983508E-9</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4.2647553194988219E-9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.251767313276311E-9</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.635411462407012E-9</v>
+      </c>
+      <c r="G7" s="3">
+        <v>6.8060963811114068E-9</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2.5668374421711841E-9</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>6.5886854093101561E-9</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>8.429864958176454</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>8.370105880426058</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>8.9024763931318756</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>8.7863729626541893</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>8.1671019051537463</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>8.5906016343295235</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>8.1812012282640172</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5.0881576180199481E-9</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.1214859842462679E-9</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7.4506099612270794E-10</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4.0698407374227369E-9</v>
+      </c>
+      <c r="G8" s="3">
+        <v>7.1129581169233448E-9</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5.0971140907863934E-9</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5.7384738911140242E-9</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>8.2934394438266121</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>8.3849461727036605</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>9.127808171285082</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>8.3904225854214118</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>8.147949748541377</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>8.2926756453117392</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>8.2412035899698317</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3.8463686825188901E-10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.9286009631696399E-10</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6.6808727730745338E-10</v>
+      </c>
+      <c r="H9" s="3">
+        <v>9.6271790097802042E-10</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.5370886086912611E-12</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>9.4149490900638622</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>9.5333397991273578</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>9.1751667986366279</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>9.0165009527473181</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>11.813301095963855</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.504451376074184E-12</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>11.822621844111286</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.212287937838473E-8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>8.7450415659962609E-9</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3.7246326398423859E-10</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3.9567658732446427E-8</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.501884418927614E-8</v>
+      </c>
+      <c r="H12" s="3">
+        <v>4.3559348943143008E-8</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3.0649464961700861E-12</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.0879066518968111E-8</v>
+      </c>
+      <c r="K12" s="3">
+        <v>9.2042064952592878E-9</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>7.9163942160092251</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>8.0582381219383166</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>9.4289165552262642</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>7.4026596467180825</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>7.8233634882062741</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>7.3609186200207954</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>11.513577102424819</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>7.9634083677861458</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="M5:U12">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(M5))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>10</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{2A0AC6FE-FA07-46EA-8716-3B4150DDCEF8}">
+            <xm:f>'pbe0 delta_E_S2_T1'!C5&lt;0.3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCCFFCC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C5:K12</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4.534643</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6.0190919999999997</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8.4928790000000003</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5.5373049999999999</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5.2642009999999999</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4.98827</v>
+      </c>
+      <c r="I5" s="5">
+        <v>9.2928990000000002</v>
+      </c>
+      <c r="J5" s="5">
+        <v>5.8396610000000004</v>
+      </c>
+      <c r="K5" s="5">
+        <v>10.118312</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1.9762299999999999</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5.1225579999999997</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7.9695320000000001</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4.542446</v>
+      </c>
+      <c r="G6" s="5">
+        <v>4.3188630000000003</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.89479200000000003</v>
+      </c>
+      <c r="I6" s="5">
+        <v>8.6520700000000001</v>
+      </c>
+      <c r="J6" s="5">
+        <v>5.0431929999999996</v>
+      </c>
+      <c r="K6" s="5">
+        <v>9.5064270000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4.130674</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5.6744490000000001</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5.9721080000000004</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5.0786360000000004</v>
+      </c>
+      <c r="G7" s="5">
+        <v>4.9314220000000004</v>
+      </c>
+      <c r="H7" s="5">
+        <v>4.8061809999999996</v>
+      </c>
+      <c r="I7" s="5">
+        <v>9.0302799999999994</v>
+      </c>
+      <c r="J7" s="5">
+        <v>5.4934229999999999</v>
+      </c>
+      <c r="K7" s="5">
+        <v>9.8412740000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3.7997749999999999</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5.1816519999999997</v>
+      </c>
+      <c r="E8" s="5">
+        <v>8.426202</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4.761933</v>
+      </c>
+      <c r="G8" s="5">
+        <v>4.4591240000000001</v>
+      </c>
+      <c r="H8" s="5">
+        <v>4.3377559999999997</v>
+      </c>
+      <c r="I8" s="5">
+        <v>8.6503460000000008</v>
+      </c>
+      <c r="J8" s="5">
+        <v>5.2752270000000001</v>
+      </c>
+      <c r="K8" s="5">
+        <v>9.4671350000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7.4539850000000003</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8.7391900000000007</v>
+      </c>
+      <c r="E9" s="5">
+        <v>9.6734609999999996</v>
+      </c>
+      <c r="F9" s="5">
+        <v>8.0035779999999992</v>
+      </c>
+      <c r="G9" s="5">
+        <v>8.1448730000000005</v>
+      </c>
+      <c r="H9" s="5">
+        <v>8.0247589999999995</v>
+      </c>
+      <c r="I9" s="5">
+        <v>9.0212380000000003</v>
+      </c>
+      <c r="J9" s="5">
+        <v>8.4405789999999996</v>
+      </c>
+      <c r="K9" s="5">
+        <v>12.89071</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5">
+        <v>7.9335019999999998</v>
+      </c>
+      <c r="D10" s="5">
+        <v>9.1400710000000007</v>
+      </c>
+      <c r="E10" s="5">
+        <v>10.530792999999999</v>
+      </c>
+      <c r="F10" s="5">
+        <v>8.2786519999999992</v>
+      </c>
+      <c r="G10" s="5">
+        <v>8.5192720000000008</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8.0998400000000004</v>
+      </c>
+      <c r="I10" s="5">
+        <v>10.045776</v>
+      </c>
+      <c r="J10" s="5">
+        <v>9.193899</v>
+      </c>
+      <c r="K10" s="5">
+        <v>10.653511999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5">
+        <v>7.6228069999999999</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8.8476300000000005</v>
+      </c>
+      <c r="E11" s="5">
+        <v>10.621302</v>
+      </c>
+      <c r="F11" s="5">
+        <v>8.1265800000000006</v>
+      </c>
+      <c r="G11" s="5">
+        <v>8.2913340000000009</v>
+      </c>
+      <c r="H11" s="5">
+        <v>8.2359019999999994</v>
+      </c>
+      <c r="I11" s="5">
+        <v>9.957929</v>
+      </c>
+      <c r="J11" s="5">
+        <v>8.6581080000000004</v>
+      </c>
+      <c r="K11" s="5">
+        <v>13.279529</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5">
+        <v>3.6444869999999998</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5.5297010000000002</v>
+      </c>
+      <c r="E12" s="5">
+        <v>8.4977359999999997</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5.2829949999999997</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4.8881290000000002</v>
+      </c>
+      <c r="H12" s="5">
+        <v>4.3187280000000001</v>
+      </c>
+      <c r="I12" s="5">
+        <v>9.0119450000000008</v>
+      </c>
+      <c r="J12" s="5">
+        <v>5.5690860000000004</v>
+      </c>
+      <c r="K12" s="5">
+        <v>10.473739999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:K12">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.23760136030000001</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.17276089980000001</v>
+      </c>
+      <c r="E5" s="6">
+        <v>5.6535188200000003E-2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.21636715949999999</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.21525722159999999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.29774262979999999</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3.1162439199999999E-2</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.1518159396</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1.4218713500000001E-2</v>
+      </c>
+      <c r="M5" s="17">
+        <f t="shared" ref="M5:M12" si="0">AVERAGE(C5:K5)</f>
+        <v>0.15482906127777779</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.63834771170000004</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.29478291919999999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.10426153959999999</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.4024552871</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.36297076230000003</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.71703173050000002</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5.4233290400000002E-2</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.26271482979999999</v>
+      </c>
+      <c r="K6" s="6">
+        <v>2.5678724199999999E-2</v>
+      </c>
+      <c r="M6" s="17">
+        <f t="shared" si="0"/>
+        <v>0.31805297720000003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.29797221010000002</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.17979402880000001</v>
+      </c>
+      <c r="E7" s="6">
+        <v>7.1358676900000001E-2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.21900476739999999</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.22078583509999999</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.2898366772</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2.9735901299999999E-2</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.17012139840000001</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1.43411562E-2</v>
+      </c>
+      <c r="M7" s="17">
+        <f t="shared" si="0"/>
+        <v>0.16588340571111113</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.36642078459999999</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.24116531869999999</v>
+      </c>
+      <c r="E8" s="6">
+        <v>7.9802534899999999E-2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.2867490009</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.2974748982</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.35510318689999998</v>
+      </c>
+      <c r="I8" s="6">
+        <v>4.2109527200000003E-2</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.21190477020000001</v>
+      </c>
+      <c r="K8" s="6">
+        <v>2.07643117E-2</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.21127714814444445</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>5.6876495899999997E-2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.72007705E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>7.9629512000000003E-3</v>
+      </c>
+      <c r="F9" s="6">
+        <v>3.8248351999999999E-2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>2.2421045899999999E-2</v>
+      </c>
+      <c r="H9" s="6">
+        <v>4.58998672E-2</v>
+      </c>
+      <c r="I9" s="6">
+        <v>4.7214672000000001E-3</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1.4164344000000001E-2</v>
+      </c>
+      <c r="K9" s="6">
+        <v>7.6479070000000002E-4</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" si="0"/>
+        <v>2.3140009399999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5.7711225599999999E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.6980774399999999E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>7.5374732999999999E-3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>4.6517446499999997E-2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2.2558970500000001E-2</v>
+      </c>
+      <c r="H10" s="6">
+        <v>6.7866556800000005E-2</v>
+      </c>
+      <c r="I10" s="6">
+        <v>3.6547045000000001E-3</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1.1860087E-2</v>
+      </c>
+      <c r="K10" s="6">
+        <v>2.7870855000000001E-3</v>
+      </c>
+      <c r="M10" s="17">
+        <f t="shared" si="0"/>
+        <v>2.638603601111111E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5.8578024499999999E-2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.6254745000000001E-2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>7.0293643000000003E-3</v>
+      </c>
+      <c r="F11" s="6">
+        <v>3.8432962799999998E-2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2.11948806E-2</v>
+      </c>
+      <c r="H11" s="6">
+        <v>4.3589417999999998E-2</v>
+      </c>
+      <c r="I11" s="6">
+        <v>4.0869762999999996E-3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1.2620908599999999E-2</v>
+      </c>
+      <c r="K11" s="6">
+        <v>2.9676149999999999E-4</v>
+      </c>
+      <c r="M11" s="17">
+        <f t="shared" si="0"/>
+        <v>2.2453782399999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.42645717649999998</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.30074245440000003</v>
+      </c>
+      <c r="E12" s="6">
+        <v>9.9601925399999999E-2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.35398097109999999</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.35422716710000002</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.49911177620000002</v>
+      </c>
+      <c r="I12" s="6">
+        <v>5.25691509E-2</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.25245390359999997</v>
+      </c>
+      <c r="K12" s="6">
+        <v>2.1508712199999998E-2</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" si="0"/>
+        <v>0.26229480415555556</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="17">
+        <f t="shared" ref="C14:K14" si="1">AVERAGE(C5:C12)</f>
+        <v>0.26749562365000001</v>
+      </c>
+      <c r="D14" s="17">
+        <f t="shared" si="1"/>
+        <v>0.15496023885000001</v>
+      </c>
+      <c r="E14" s="17">
+        <f t="shared" si="1"/>
+        <v>5.4261206724999997E-2</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="1"/>
+        <v>0.20021949341249998</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="1"/>
+        <v>0.18961134766249998</v>
+      </c>
+      <c r="H14" s="17">
+        <f t="shared" si="1"/>
+        <v>0.28952273032500003</v>
+      </c>
+      <c r="I14" s="17">
+        <f t="shared" si="1"/>
+        <v>2.7784182124999997E-2</v>
+      </c>
+      <c r="J14" s="17">
+        <f t="shared" si="1"/>
+        <v>0.13595702264999998</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="1"/>
+        <v>1.2545031937499999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:K12">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:M12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:K14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.2602889999999999E-4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6.3695399999999993E-5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7.8815999999999992E-6</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9.7062699999999995E-5</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.110645E-4</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.890971E-4</v>
+      </c>
+      <c r="I5" s="3">
+        <v>6.8853E-6</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5.8160800000000001E-5</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.0640000000000001E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7.115496E-4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.056812E-4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.9183000000000002E-5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.1302430000000001E-4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.4782770000000001E-4</v>
+      </c>
+      <c r="H6" s="3">
+        <v>8.6165320000000005E-4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.0811599999999999E-5</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.857966E-4</v>
+      </c>
+      <c r="K6" s="3">
+        <v>3.5885E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.9982809999999999E-4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7.0969099999999998E-5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.02932E-5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.024563E-4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.170149E-4</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1.747614E-4</v>
+      </c>
+      <c r="I7" s="3">
+        <v>5.8528000000000001E-6</v>
+      </c>
+      <c r="J7" s="3">
+        <v>7.1956299999999994E-5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1.043E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.4522300000000003E-4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.3694010000000001E-4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.1067300000000001E-5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.961551E-4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.29941E-4</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2.999314E-4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.2481599999999999E-5</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.1548010000000001E-4</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2.3740000000000001E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8.5835000000000001E-6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5.9260000000000005E-7</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.2809999999999999E-7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.7184999999999999E-6</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1.0954999999999999E-6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4.9405000000000004E-6</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5.8899999999999998E-8</v>
+      </c>
+      <c r="J9" s="3">
+        <v>4.6839999999999999E-7</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.9000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8.4013000000000004E-6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5.1490000000000004E-7</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.0700000000000001E-7</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4.9342000000000001E-6</v>
+      </c>
+      <c r="G10" s="3">
+        <v>9.794000000000001E-7</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.0784E-5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3.9500000000000003E-8</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3.0470000000000002E-7</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2.18E-8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9.6647999999999994E-6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6.1610000000000002E-7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.038E-7</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3.6921000000000002E-6</v>
+      </c>
+      <c r="G11" s="3">
+        <v>9.9260000000000003E-7</v>
+      </c>
+      <c r="H11" s="3">
+        <v>4.7454999999999997E-6</v>
+      </c>
+      <c r="I11" s="3">
+        <v>5.1E-8</v>
+      </c>
+      <c r="J11" s="3">
+        <v>4.0499999999999999E-7</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3E-10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.6968630000000002E-4</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.0533300000000001E-4</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3.6794700000000002E-5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3.0858710000000001E-4</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3.144981E-4</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5.4324470000000004E-4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.0593200000000001E-5</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.68918E-4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2.8044000000000002E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K12"/>
@@ -4386,18 +7520,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -4730,18 +7864,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -5074,18 +8208,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -5418,18 +8552,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -5762,18 +8896,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -6097,7 +9231,7 @@
   <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6106,18 +9240,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -6441,7 +9575,7 @@
   <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6450,18 +9584,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>

</xml_diff>